<commit_message>
Fixed Microcode Cheat Sheet_experimental.xlsx
</commit_message>
<xml_diff>
--- a/software/prime_number_experimental/Microcode Cheat Sheet_experimental.xlsx
+++ b/software/prime_number_experimental/Microcode Cheat Sheet_experimental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\eater_8bit\eater-8bit-cpu-programmer\software\prime_number_experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1551023-CED1-4B19-9444-2CAB4AEEDC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8028276B-7933-48E3-BED4-51ADE32E27BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{096FE876-D004-418E-87BD-E4E231232AC4}"/>
+    <workbookView xWindow="13260" yWindow="3030" windowWidth="13605" windowHeight="11580" xr2:uid="{096FE876-D004-418E-87BD-E4E231232AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Microcodes" sheetId="1" r:id="rId1"/>
@@ -131,21 +131,12 @@
     <t>DSP</t>
   </si>
   <si>
-    <t>Decrement: Similar to INC, subtract a specified 4-bit number directly from what’s in the A register.</t>
-  </si>
-  <si>
-    <t>Increment: Add a specified 4-bit number directly to what’s in the A register. Saves from having to use a memory address to store a 1 (or other number) to count up and down by.</t>
-  </si>
-  <si>
     <t>Jump if Not Zero: Jump to program counter step if Zero Flag is not set</t>
   </si>
   <si>
     <t>Jump if Not Carry: Jump to program counter step if Carry Flag is not set</t>
   </si>
   <si>
-    <t>Display and Halt: Outputs the value at a specified memory address to the screen and halt.</t>
-  </si>
-  <si>
     <t>w 51 48 E0 28 70 E0 48 63</t>
   </si>
   <si>
@@ -195,6 +186,15 @@
   </si>
   <si>
     <t>Description: Test ADDS instraction</t>
+  </si>
+  <si>
+    <t>Decrement: Subtract a specified 4-bit number directly from what’s in the A register.</t>
+  </si>
+  <si>
+    <t>Display: Outputs the value at a specified memory address to the screen.</t>
+  </si>
+  <si>
+    <t>Add: Take value stored at instruction pointer address, load into B register, add and output to bus, load into A register and store at the instruction pointer address.</t>
   </si>
 </sst>
 </file>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610C6AD0-1FF4-4D5A-A084-2817C748181F}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +728,7 @@
         <v>1001</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,18 +739,18 @@
         <v>1010</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
         <v>1011</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>1100</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>1101</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,18 +783,18 @@
         <v>1110</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" s="5">
         <v>1111</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -813,13 +813,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F656228-CF52-49E8-83BA-5599FD8BE868}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -883,13 +885,13 @@
         <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -897,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -1025,7 +1027,7 @@
         <v>1F</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -1062,7 +1064,7 @@
         <v>3E</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K9">
         <v>5</v>
@@ -1175,7 +1177,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -1368,7 +1370,7 @@
         <v>00</v>
       </c>
       <c r="J18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K18">
         <v>14</v>
@@ -1402,7 +1404,7 @@
         <v>02</v>
       </c>
       <c r="J19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K19">
         <v>15</v>
@@ -2491,7 +2493,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2561,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4">
         <v>15</v>
@@ -2747,7 +2749,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3005,7 +3007,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3074,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4">
         <v>15</v>
@@ -3505,7 +3507,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3569,7 +3571,7 @@
         <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4006,7 +4008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9203E6-3A82-4AC0-9C5C-BBEDFA9126D1}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -4014,7 +4016,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4086,7 +4088,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4">
         <v>13</v>
@@ -4155,7 +4157,7 @@
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L6" s="4">
         <v>13</v>
@@ -4446,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="str">
         <f t="shared" si="1"/>
@@ -4512,7 +4514,7 @@
         <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -4681,7 +4683,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>